<commit_message>
add bug reports, refactor
</commit_message>
<xml_diff>
--- a/akvelon.xlsx
+++ b/akvelon.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Парковка" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="199">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -473,15 +473,6 @@
   </si>
   <si>
     <t>NA</t>
-  </si>
-  <si>
-    <t>#1</t>
-  </si>
-  <si>
-    <t>#2</t>
-  </si>
-  <si>
-    <t>#3</t>
   </si>
   <si>
     <t>Значения сигналов:        
@@ -982,7 +973,10 @@
     <t>8. Neutral</t>
   </si>
   <si>
-    <t>11. Park</t>
+    <t>9. Park</t>
+  </si>
+  <si>
+    <t>10. Neutral</t>
   </si>
   <si>
     <t>Gear_1 = 0.67V
@@ -1025,9 +1019,6 @@
 AccPedal = 3.49V
 BrakePedal = 2V
 BatteryVoltage = 800.0V</t>
-  </si>
-  <si>
-    <t>12. Neutral</t>
   </si>
   <si>
     <t>Имитируется холостой ход: машина в режиме паркинга или  нейтрали, подается постепенно газ</t>
@@ -1039,6 +1030,65 @@
 BrakePedalState: Released
 ReqTorque: 0 Nm
 BatteryState: Ready</t>
+  </si>
+  <si>
+    <t>Значения сигналов:        
+GearPosition: Park 
+AccPedalPos: 50 %
+BrakePedalState: Released
+ReqTorque: 5000 Nm
+BatteryState: Ready</t>
+  </si>
+  <si>
+    <t>Значения сигналов:        
+GearPosition: Park 
+AccPedalPos: 30 %
+BrakePedalState: Released
+ReqTorque: 0 Nm
+BatteryState: Ready</t>
+  </si>
+  <si>
+    <t>Значения сигналов:        
+GearPosition: Neutral
+AccPedalPos: 30 %
+BrakePedalState: Released
+ReqTorque: 0 Nm
+BatteryState: Ready</t>
+  </si>
+  <si>
+    <t>Значения сигналов:        
+GearPosition: Neutral 
+AccPedalPos: 100 %
+BrakePedalState: Released
+ReqTorque: 0 Nm
+BatteryState: Ready</t>
+  </si>
+  <si>
+    <t>Значения сигналов:        
+GearPosition: Park 
+AccPedalPos: 100 %
+BrakePedalState: Released
+ReqTorque: 0 Nm
+BatteryState: Ready</t>
+  </si>
+  <si>
+    <t>Значения сигналов:        
+GearPosition: Neutral 
+AccPedalPos: 50 %
+BrakePedalState: Released
+ReqTorque: 0 Nm
+BatteryState: Ready</t>
+  </si>
+  <si>
+    <t>Значения сигналов:        
+GearPosition: Park 
+AccPedalPos: 50 %
+BrakePedalState: Released
+ReqTorque: 0 Nm
+BatteryState: Ready</t>
+  </si>
+  <si>
+    <t>TBD</t>
   </si>
 </sst>
 </file>
@@ -1149,7 +1199,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1242,38 +1292,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1412,9 +1436,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1448,15 +1469,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
@@ -1744,7 +1756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G9" sqref="G9:K9"/>
     </sheetView>
   </sheetViews>
@@ -2287,7 +2299,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G10" sqref="G10:K10"/>
     </sheetView>
   </sheetViews>
@@ -2840,10 +2852,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N43"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32:H32"/>
+    <sheetView topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O46" sqref="O46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3044,7 +3056,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="5"/>
@@ -3155,7 +3167,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="47"/>
     </row>
-    <row r="17" spans="1:14" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="27"/>
       <c r="B17" s="43"/>
       <c r="C17" s="44"/>
@@ -3173,7 +3185,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="47"/>
     </row>
-    <row r="18" spans="1:14" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="27"/>
       <c r="B18" s="43"/>
       <c r="C18" s="44"/>
@@ -3193,7 +3205,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="27"/>
       <c r="B19" s="43"/>
       <c r="C19" s="44"/>
@@ -3211,7 +3223,7 @@
       <c r="K19" s="5"/>
       <c r="L19" s="47"/>
     </row>
-    <row r="20" spans="1:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="27"/>
       <c r="B20" s="43"/>
       <c r="C20" s="44"/>
@@ -3229,7 +3241,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="47"/>
     </row>
-    <row r="21" spans="1:14" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="27"/>
       <c r="B21" s="43"/>
       <c r="C21" s="44"/>
@@ -3249,7 +3261,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="27"/>
       <c r="B22" s="43"/>
       <c r="C22" s="44"/>
@@ -3267,7 +3279,7 @@
       <c r="K22" s="5"/>
       <c r="L22" s="47"/>
     </row>
-    <row r="23" spans="1:14" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="27"/>
       <c r="B23" s="43"/>
       <c r="C23" s="44"/>
@@ -3285,7 +3297,7 @@
       <c r="K23" s="5"/>
       <c r="L23" s="47"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -3298,12 +3310,12 @@
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
     </row>
-    <row r="25" spans="1:14" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="29" t="s">
         <v>16</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C25" s="31"/>
       <c r="D25" s="31"/>
@@ -3315,7 +3327,7 @@
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="32"/>
       <c r="B26" s="32"/>
       <c r="C26" s="32"/>
@@ -3328,7 +3340,7 @@
       <c r="J26" s="32"/>
       <c r="K26" s="32"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="33" t="s">
         <v>17</v>
       </c>
@@ -3350,13 +3362,8 @@
       </c>
       <c r="J27" s="37"/>
       <c r="K27" s="37"/>
-      <c r="L27" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="M27" s="37"/>
-      <c r="N27" s="37"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="34"/>
       <c r="B28" s="38"/>
       <c r="C28" s="38"/>
@@ -3368,11 +3375,8 @@
       <c r="I28" s="37"/>
       <c r="J28" s="37"/>
       <c r="K28" s="37"/>
-      <c r="L28" s="37"/>
-      <c r="M28" s="37"/>
-      <c r="N28" s="37"/>
-    </row>
-    <row r="29" spans="1:14" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:12" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="27">
         <v>1</v>
       </c>
@@ -3394,18 +3398,13 @@
       </c>
       <c r="J29" s="4"/>
       <c r="K29" s="5"/>
-      <c r="L29" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="M29" s="50"/>
-      <c r="N29" s="51"/>
-    </row>
-    <row r="30" spans="1:14" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:12" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="27">
         <v>2</v>
       </c>
       <c r="B30" s="39" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C30" s="40"/>
       <c r="D30" s="39" t="s">
@@ -3422,18 +3421,13 @@
       </c>
       <c r="J30" s="4"/>
       <c r="K30" s="5"/>
-      <c r="L30" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="M30" s="50"/>
-      <c r="N30" s="51"/>
-    </row>
-    <row r="31" spans="1:14" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:12" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="27">
         <v>3</v>
       </c>
       <c r="B31" s="39" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C31" s="40"/>
       <c r="D31" s="39" t="s">
@@ -3450,26 +3444,21 @@
       </c>
       <c r="J31" s="4"/>
       <c r="K31" s="5"/>
-      <c r="L31" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="M31" s="50"/>
-      <c r="N31" s="51"/>
-    </row>
-    <row r="32" spans="1:14" ht="119.4" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:12" ht="119.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="27">
         <v>4</v>
       </c>
       <c r="B32" s="39" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C32" s="40"/>
       <c r="D32" s="39" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E32" s="39"/>
       <c r="F32" s="28" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="5"/>
@@ -3478,26 +3467,21 @@
       </c>
       <c r="J32" s="4"/>
       <c r="K32" s="5"/>
-      <c r="L32" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="M32" s="50"/>
-      <c r="N32" s="51"/>
-    </row>
-    <row r="33" spans="1:14" ht="97.8" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:11" ht="97.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="27">
         <v>5</v>
       </c>
       <c r="B33" s="39" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C33" s="40"/>
       <c r="D33" s="39" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E33" s="39"/>
       <c r="F33" s="28" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="5"/>
@@ -3506,13 +3490,8 @@
       </c>
       <c r="J33" s="4"/>
       <c r="K33" s="5"/>
-      <c r="L33" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="M33" s="50"/>
-      <c r="N33" s="51"/>
-    </row>
-    <row r="34" spans="1:14" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:11" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="27">
         <v>6</v>
       </c>
@@ -3521,11 +3500,11 @@
       </c>
       <c r="C34" s="40"/>
       <c r="D34" s="39" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E34" s="39"/>
       <c r="F34" s="28" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="5"/>
@@ -3534,13 +3513,8 @@
       </c>
       <c r="J34" s="4"/>
       <c r="K34" s="5"/>
-      <c r="L34" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="M34" s="50"/>
-      <c r="N34" s="51"/>
-    </row>
-    <row r="35" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="27">
         <v>7</v>
       </c>
@@ -3562,13 +3536,8 @@
       </c>
       <c r="J35" s="4"/>
       <c r="K35" s="5"/>
-      <c r="L35" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="M35" s="50"/>
-      <c r="N35" s="51"/>
-    </row>
-    <row r="36" spans="1:14" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:11" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="27">
         <v>8</v>
       </c>
@@ -3590,18 +3559,13 @@
       </c>
       <c r="J36" s="4"/>
       <c r="K36" s="5"/>
-      <c r="L36" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="M36" s="50"/>
-      <c r="N36" s="51"/>
-    </row>
-    <row r="37" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="27">
         <v>9</v>
       </c>
       <c r="B37" s="39" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C37" s="40"/>
       <c r="D37" s="39" t="s">
@@ -3618,18 +3582,13 @@
       </c>
       <c r="J37" s="4"/>
       <c r="K37" s="5"/>
-      <c r="L37" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="M37" s="50"/>
-      <c r="N37" s="51"/>
-    </row>
-    <row r="38" spans="1:14" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:11" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="27">
         <v>10</v>
       </c>
       <c r="B38" s="39" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C38" s="40"/>
       <c r="D38" s="39" t="s">
@@ -3646,18 +3605,13 @@
       </c>
       <c r="J38" s="4"/>
       <c r="K38" s="5"/>
-      <c r="L38" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="M38" s="50"/>
-      <c r="N38" s="51"/>
-    </row>
-    <row r="39" spans="1:14" ht="67.8" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:11" ht="67.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="27">
         <v>11</v>
       </c>
       <c r="B39" s="39" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C39" s="40"/>
       <c r="D39" s="39" t="s">
@@ -3674,18 +3628,13 @@
       </c>
       <c r="J39" s="4"/>
       <c r="K39" s="5"/>
-      <c r="L39" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="M39" s="50"/>
-      <c r="N39" s="51"/>
-    </row>
-    <row r="40" spans="1:14" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:11" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="27">
         <v>12</v>
       </c>
       <c r="B40" s="39" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C40" s="40"/>
       <c r="D40" s="39" t="s">
@@ -3702,18 +3651,13 @@
       </c>
       <c r="J40" s="4"/>
       <c r="K40" s="5"/>
-      <c r="L40" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="M40" s="50"/>
-      <c r="N40" s="51"/>
-    </row>
-    <row r="41" spans="1:14" ht="70.8" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:11" ht="70.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="27">
         <v>13</v>
       </c>
       <c r="B41" s="39" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C41" s="40"/>
       <c r="D41" s="39" t="s">
@@ -3721,7 +3665,7 @@
       </c>
       <c r="E41" s="39"/>
       <c r="F41" s="28" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G41" s="4"/>
       <c r="H41" s="5"/>
@@ -3730,18 +3674,13 @@
       </c>
       <c r="J41" s="4"/>
       <c r="K41" s="5"/>
-      <c r="L41" s="46" t="s">
-        <v>94</v>
-      </c>
-      <c r="M41" s="4"/>
-      <c r="N41" s="5"/>
-    </row>
-    <row r="42" spans="1:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:11" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="27">
         <v>14</v>
       </c>
       <c r="B42" s="39" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C42" s="40"/>
       <c r="D42" s="39" t="s">
@@ -3749,7 +3688,7 @@
       </c>
       <c r="E42" s="39"/>
       <c r="F42" s="28" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G42" s="4"/>
       <c r="H42" s="5"/>
@@ -3758,18 +3697,13 @@
       </c>
       <c r="J42" s="4"/>
       <c r="K42" s="5"/>
-      <c r="L42" s="46" t="s">
-        <v>95</v>
-      </c>
-      <c r="M42" s="4"/>
-      <c r="N42" s="5"/>
-    </row>
-    <row r="43" spans="1:14" ht="76.8" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:11" ht="76.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="27">
         <v>15</v>
       </c>
       <c r="B43" s="39" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C43" s="40"/>
       <c r="D43" s="39" t="s">
@@ -3777,7 +3711,7 @@
       </c>
       <c r="E43" s="39"/>
       <c r="F43" s="28" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="5"/>
@@ -3786,33 +3720,12 @@
       </c>
       <c r="J43" s="4"/>
       <c r="K43" s="5"/>
-      <c r="L43" s="46" t="s">
-        <v>96</v>
-      </c>
-      <c r="M43" s="4"/>
-      <c r="N43" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="119">
-    <mergeCell ref="L43:N43"/>
-    <mergeCell ref="L37:N37"/>
-    <mergeCell ref="L38:N38"/>
-    <mergeCell ref="L39:N39"/>
-    <mergeCell ref="L40:N40"/>
-    <mergeCell ref="L41:N41"/>
-    <mergeCell ref="L42:N42"/>
-    <mergeCell ref="L31:N31"/>
-    <mergeCell ref="L32:N32"/>
-    <mergeCell ref="L33:N33"/>
-    <mergeCell ref="L34:N34"/>
-    <mergeCell ref="L35:N35"/>
-    <mergeCell ref="L36:N36"/>
+  <mergeCells count="103">
     <mergeCell ref="L21:L23"/>
     <mergeCell ref="G21:K21"/>
     <mergeCell ref="G22:K22"/>
-    <mergeCell ref="L27:N28"/>
-    <mergeCell ref="L29:N29"/>
-    <mergeCell ref="L30:N30"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="F42:H42"/>
@@ -3921,10 +3834,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N43"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41:K41"/>
+    <sheetView topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P42" sqref="P42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4088,7 +4001,7 @@
         <v>26</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -4112,7 +4025,7 @@
         <v>27</v>
       </c>
       <c r="G10" s="28" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -4123,7 +4036,7 @@
     <row r="11" spans="1:12" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="27"/>
       <c r="B11" s="28" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="5"/>
@@ -4132,7 +4045,7 @@
         <v>28</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -4150,7 +4063,7 @@
         <v>37</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -4170,7 +4083,7 @@
         <v>38</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
@@ -4188,7 +4101,7 @@
         <v>39</v>
       </c>
       <c r="G14" s="28" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
@@ -4206,7 +4119,7 @@
         <v>37</v>
       </c>
       <c r="G15" s="28" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
@@ -4226,7 +4139,7 @@
         <v>38</v>
       </c>
       <c r="G16" s="28" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -4234,7 +4147,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="47"/>
     </row>
-    <row r="17" spans="1:14" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="27"/>
       <c r="B17" s="43"/>
       <c r="C17" s="44"/>
@@ -4244,7 +4157,7 @@
         <v>39</v>
       </c>
       <c r="G17" s="28" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
@@ -4252,7 +4165,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="47"/>
     </row>
-    <row r="18" spans="1:14" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="27"/>
       <c r="B18" s="43"/>
       <c r="C18" s="44"/>
@@ -4262,7 +4175,7 @@
         <v>77</v>
       </c>
       <c r="G18" s="28" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
@@ -4272,7 +4185,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="27"/>
       <c r="B19" s="43"/>
       <c r="C19" s="44"/>
@@ -4282,7 +4195,7 @@
         <v>78</v>
       </c>
       <c r="G19" s="28" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
@@ -4290,7 +4203,7 @@
       <c r="K19" s="5"/>
       <c r="L19" s="47"/>
     </row>
-    <row r="20" spans="1:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="27"/>
       <c r="B20" s="43"/>
       <c r="C20" s="44"/>
@@ -4300,7 +4213,7 @@
         <v>79</v>
       </c>
       <c r="G20" s="28" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
@@ -4308,7 +4221,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="47"/>
     </row>
-    <row r="21" spans="1:14" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="27"/>
       <c r="B21" s="43"/>
       <c r="C21" s="44"/>
@@ -4318,7 +4231,7 @@
         <v>86</v>
       </c>
       <c r="G21" s="28" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
@@ -4328,7 +4241,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="27"/>
       <c r="B22" s="43"/>
       <c r="C22" s="44"/>
@@ -4338,7 +4251,7 @@
         <v>87</v>
       </c>
       <c r="G22" s="28" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
@@ -4346,7 +4259,7 @@
       <c r="K22" s="5"/>
       <c r="L22" s="47"/>
     </row>
-    <row r="23" spans="1:14" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="27"/>
       <c r="B23" s="43"/>
       <c r="C23" s="44"/>
@@ -4356,7 +4269,7 @@
         <v>88</v>
       </c>
       <c r="G23" s="28" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
@@ -4364,7 +4277,7 @@
       <c r="K23" s="5"/>
       <c r="L23" s="47"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -4377,7 +4290,7 @@
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
     </row>
-    <row r="25" spans="1:14" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="29" t="s">
         <v>16</v>
       </c>
@@ -4394,7 +4307,7 @@
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="32"/>
       <c r="B26" s="32"/>
       <c r="C26" s="32"/>
@@ -4407,7 +4320,7 @@
       <c r="J26" s="32"/>
       <c r="K26" s="32"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="33" t="s">
         <v>17</v>
       </c>
@@ -4429,13 +4342,8 @@
       </c>
       <c r="J27" s="37"/>
       <c r="K27" s="37"/>
-      <c r="L27" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="M27" s="37"/>
-      <c r="N27" s="37"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="34"/>
       <c r="B28" s="38"/>
       <c r="C28" s="38"/>
@@ -4447,11 +4355,8 @@
       <c r="I28" s="37"/>
       <c r="J28" s="37"/>
       <c r="K28" s="37"/>
-      <c r="L28" s="37"/>
-      <c r="M28" s="37"/>
-      <c r="N28" s="37"/>
-    </row>
-    <row r="29" spans="1:14" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:12" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="27">
         <v>1</v>
       </c>
@@ -4460,11 +4365,11 @@
       </c>
       <c r="C29" s="40"/>
       <c r="D29" s="39" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E29" s="39"/>
       <c r="F29" s="41" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="5"/>
@@ -4473,13 +4378,8 @@
       </c>
       <c r="J29" s="4"/>
       <c r="K29" s="5"/>
-      <c r="L29" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="M29" s="50"/>
-      <c r="N29" s="51"/>
-    </row>
-    <row r="30" spans="1:14" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:12" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="27">
         <v>2</v>
       </c>
@@ -4488,11 +4388,11 @@
       </c>
       <c r="C30" s="40"/>
       <c r="D30" s="39" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E30" s="39"/>
       <c r="F30" s="28" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="5"/>
@@ -4501,13 +4401,8 @@
       </c>
       <c r="J30" s="4"/>
       <c r="K30" s="5"/>
-      <c r="L30" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="M30" s="50"/>
-      <c r="N30" s="51"/>
-    </row>
-    <row r="31" spans="1:14" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:12" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="27">
         <v>3</v>
       </c>
@@ -4516,11 +4411,11 @@
       </c>
       <c r="C31" s="40"/>
       <c r="D31" s="39" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E31" s="39"/>
       <c r="F31" s="28" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="5"/>
@@ -4529,13 +4424,8 @@
       </c>
       <c r="J31" s="4"/>
       <c r="K31" s="5"/>
-      <c r="L31" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="M31" s="50"/>
-      <c r="N31" s="51"/>
-    </row>
-    <row r="32" spans="1:14" ht="119.4" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:12" ht="119.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="27">
         <v>4</v>
       </c>
@@ -4544,11 +4434,11 @@
       </c>
       <c r="C32" s="40"/>
       <c r="D32" s="39" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E32" s="39"/>
       <c r="F32" s="28" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="5"/>
@@ -4557,13 +4447,8 @@
       </c>
       <c r="J32" s="4"/>
       <c r="K32" s="5"/>
-      <c r="L32" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="M32" s="50"/>
-      <c r="N32" s="51"/>
-    </row>
-    <row r="33" spans="1:14" ht="97.8" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:11" ht="97.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="27">
         <v>5</v>
       </c>
@@ -4572,11 +4457,11 @@
       </c>
       <c r="C33" s="40"/>
       <c r="D33" s="39" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E33" s="39"/>
       <c r="F33" s="28" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="5"/>
@@ -4585,13 +4470,8 @@
       </c>
       <c r="J33" s="4"/>
       <c r="K33" s="5"/>
-      <c r="L33" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="M33" s="50"/>
-      <c r="N33" s="51"/>
-    </row>
-    <row r="34" spans="1:14" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:11" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="27">
         <v>6</v>
       </c>
@@ -4613,13 +4493,8 @@
       </c>
       <c r="J34" s="4"/>
       <c r="K34" s="5"/>
-      <c r="L34" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="M34" s="50"/>
-      <c r="N34" s="51"/>
-    </row>
-    <row r="35" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="27">
         <v>7</v>
       </c>
@@ -4628,11 +4503,11 @@
       </c>
       <c r="C35" s="40"/>
       <c r="D35" s="39" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E35" s="39"/>
       <c r="F35" s="28" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G35" s="4"/>
       <c r="H35" s="5"/>
@@ -4641,13 +4516,8 @@
       </c>
       <c r="J35" s="4"/>
       <c r="K35" s="5"/>
-      <c r="L35" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="M35" s="50"/>
-      <c r="N35" s="51"/>
-    </row>
-    <row r="36" spans="1:14" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:11" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="27">
         <v>8</v>
       </c>
@@ -4656,11 +4526,11 @@
       </c>
       <c r="C36" s="40"/>
       <c r="D36" s="39" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E36" s="39"/>
       <c r="F36" s="28" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G36" s="4"/>
       <c r="H36" s="5"/>
@@ -4669,13 +4539,8 @@
       </c>
       <c r="J36" s="4"/>
       <c r="K36" s="5"/>
-      <c r="L36" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="M36" s="50"/>
-      <c r="N36" s="51"/>
-    </row>
-    <row r="37" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="27">
         <v>9</v>
       </c>
@@ -4684,11 +4549,11 @@
       </c>
       <c r="C37" s="40"/>
       <c r="D37" s="39" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E37" s="39"/>
       <c r="F37" s="28" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G37" s="4"/>
       <c r="H37" s="5"/>
@@ -4697,13 +4562,8 @@
       </c>
       <c r="J37" s="4"/>
       <c r="K37" s="5"/>
-      <c r="L37" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="M37" s="50"/>
-      <c r="N37" s="51"/>
-    </row>
-    <row r="38" spans="1:14" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:11" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="27">
         <v>10</v>
       </c>
@@ -4712,11 +4572,11 @@
       </c>
       <c r="C38" s="40"/>
       <c r="D38" s="39" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E38" s="39"/>
       <c r="F38" s="28" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G38" s="4"/>
       <c r="H38" s="5"/>
@@ -4725,13 +4585,8 @@
       </c>
       <c r="J38" s="4"/>
       <c r="K38" s="5"/>
-      <c r="L38" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="M38" s="50"/>
-      <c r="N38" s="51"/>
-    </row>
-    <row r="39" spans="1:14" ht="67.8" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:11" ht="67.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="27">
         <v>11</v>
       </c>
@@ -4740,11 +4595,11 @@
       </c>
       <c r="C39" s="40"/>
       <c r="D39" s="39" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E39" s="39"/>
       <c r="F39" s="28" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G39" s="4"/>
       <c r="H39" s="5"/>
@@ -4753,13 +4608,8 @@
       </c>
       <c r="J39" s="4"/>
       <c r="K39" s="5"/>
-      <c r="L39" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="M39" s="50"/>
-      <c r="N39" s="51"/>
-    </row>
-    <row r="40" spans="1:14" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:11" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="27">
         <v>12</v>
       </c>
@@ -4768,11 +4618,11 @@
       </c>
       <c r="C40" s="40"/>
       <c r="D40" s="39" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E40" s="39"/>
       <c r="F40" s="28" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G40" s="4"/>
       <c r="H40" s="5"/>
@@ -4781,13 +4631,8 @@
       </c>
       <c r="J40" s="4"/>
       <c r="K40" s="5"/>
-      <c r="L40" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="M40" s="50"/>
-      <c r="N40" s="51"/>
-    </row>
-    <row r="41" spans="1:14" ht="70.8" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:11" ht="70.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="27">
         <v>13</v>
       </c>
@@ -4796,11 +4641,11 @@
       </c>
       <c r="C41" s="40"/>
       <c r="D41" s="39" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E41" s="39"/>
       <c r="F41" s="28" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G41" s="4"/>
       <c r="H41" s="5"/>
@@ -4809,13 +4654,8 @@
       </c>
       <c r="J41" s="4"/>
       <c r="K41" s="5"/>
-      <c r="L41" s="46" t="s">
-        <v>94</v>
-      </c>
-      <c r="M41" s="4"/>
-      <c r="N41" s="5"/>
-    </row>
-    <row r="42" spans="1:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:11" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="27">
         <v>14</v>
       </c>
@@ -4824,11 +4664,11 @@
       </c>
       <c r="C42" s="40"/>
       <c r="D42" s="39" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E42" s="39"/>
       <c r="F42" s="28" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G42" s="4"/>
       <c r="H42" s="5"/>
@@ -4837,13 +4677,8 @@
       </c>
       <c r="J42" s="4"/>
       <c r="K42" s="5"/>
-      <c r="L42" s="46" t="s">
-        <v>95</v>
-      </c>
-      <c r="M42" s="4"/>
-      <c r="N42" s="5"/>
-    </row>
-    <row r="43" spans="1:14" ht="76.8" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:11" ht="76.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="27">
         <v>15</v>
       </c>
@@ -4852,11 +4687,11 @@
       </c>
       <c r="C43" s="40"/>
       <c r="D43" s="39" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E43" s="39"/>
       <c r="F43" s="28" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="5"/>
@@ -4865,90 +4700,69 @@
       </c>
       <c r="J43" s="4"/>
       <c r="K43" s="5"/>
-      <c r="L43" s="46" t="s">
-        <v>96</v>
-      </c>
-      <c r="M43" s="4"/>
-      <c r="N43" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="119">
+  <mergeCells count="103">
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="F42:H42"/>
     <mergeCell ref="I42:K42"/>
-    <mergeCell ref="L42:N42"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="D43:E43"/>
     <mergeCell ref="F43:H43"/>
     <mergeCell ref="I43:K43"/>
-    <mergeCell ref="L43:N43"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="D40:E40"/>
     <mergeCell ref="F40:H40"/>
     <mergeCell ref="I40:K40"/>
-    <mergeCell ref="L40:N40"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="D41:E41"/>
     <mergeCell ref="F41:H41"/>
     <mergeCell ref="I41:K41"/>
-    <mergeCell ref="L41:N41"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="D38:E38"/>
     <mergeCell ref="F38:H38"/>
     <mergeCell ref="I38:K38"/>
-    <mergeCell ref="L38:N38"/>
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="F39:H39"/>
     <mergeCell ref="I39:K39"/>
-    <mergeCell ref="L39:N39"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="F36:H36"/>
     <mergeCell ref="I36:K36"/>
-    <mergeCell ref="L36:N36"/>
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="D37:E37"/>
     <mergeCell ref="F37:H37"/>
     <mergeCell ref="I37:K37"/>
-    <mergeCell ref="L37:N37"/>
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="F34:H34"/>
     <mergeCell ref="I34:K34"/>
-    <mergeCell ref="L34:N34"/>
     <mergeCell ref="B35:C35"/>
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="F35:H35"/>
     <mergeCell ref="I35:K35"/>
-    <mergeCell ref="L35:N35"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="F32:H32"/>
     <mergeCell ref="I32:K32"/>
-    <mergeCell ref="L32:N32"/>
     <mergeCell ref="B33:C33"/>
     <mergeCell ref="D33:E33"/>
     <mergeCell ref="F33:H33"/>
     <mergeCell ref="I33:K33"/>
-    <mergeCell ref="L33:N33"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="F30:H30"/>
     <mergeCell ref="I30:K30"/>
-    <mergeCell ref="L30:N30"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="F31:H31"/>
     <mergeCell ref="I31:K31"/>
-    <mergeCell ref="L31:N31"/>
-    <mergeCell ref="L27:N28"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="I29:K29"/>
-    <mergeCell ref="L29:N29"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="B27:C28"/>
@@ -5002,8 +4816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30:E30"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5164,7 +4978,7 @@
       <c r="D9" s="5"/>
       <c r="E9" s="8"/>
       <c r="F9" s="27" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G9" s="28" t="s">
         <v>41</v>
@@ -5173,7 +4987,7 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="5"/>
-      <c r="L9" s="64" t="s">
+      <c r="L9" s="60" t="s">
         <v>49</v>
       </c>
     </row>
@@ -5188,7 +5002,7 @@
       <c r="D10" s="5"/>
       <c r="E10" s="8"/>
       <c r="F10" s="27" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G10" s="28" t="s">
         <v>44</v>
@@ -5197,7 +5011,7 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="5"/>
-      <c r="L10" s="64"/>
+      <c r="L10" s="60"/>
     </row>
     <row r="11" spans="1:12" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="27"/>
@@ -5206,7 +5020,7 @@
       <c r="D11" s="45"/>
       <c r="E11" s="8"/>
       <c r="F11" s="27" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G11" s="28" t="s">
         <v>60</v>
@@ -5215,7 +5029,7 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="5"/>
-      <c r="L11" s="64" t="s">
+      <c r="L11" s="60" t="s">
         <v>63</v>
       </c>
     </row>
@@ -5226,7 +5040,7 @@
       <c r="D12" s="45"/>
       <c r="E12" s="8"/>
       <c r="F12" s="27" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="G12" s="28" t="s">
         <v>47</v>
@@ -5235,7 +5049,7 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="5"/>
-      <c r="L12" s="64"/>
+      <c r="L12" s="60"/>
     </row>
     <row r="13" spans="1:12" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="27"/>
@@ -5244,16 +5058,16 @@
       <c r="D13" s="45"/>
       <c r="E13" s="8"/>
       <c r="F13" s="27" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="5"/>
-      <c r="L13" s="64" t="s">
+      <c r="L13" s="60" t="s">
         <v>64</v>
       </c>
     </row>
@@ -5264,16 +5078,16 @@
       <c r="D14" s="45"/>
       <c r="E14" s="8"/>
       <c r="F14" s="27" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="G14" s="28" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="5"/>
-      <c r="L14" s="64"/>
+      <c r="L14" s="60"/>
     </row>
     <row r="15" spans="1:12" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="27"/>
@@ -5282,16 +5096,16 @@
       <c r="D15" s="45"/>
       <c r="E15" s="8"/>
       <c r="F15" s="27" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G15" s="28" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="5"/>
-      <c r="L15" s="64" t="s">
+      <c r="L15" s="60" t="s">
         <v>84</v>
       </c>
     </row>
@@ -5302,16 +5116,16 @@
       <c r="D16" s="45"/>
       <c r="E16" s="8"/>
       <c r="F16" s="27" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G16" s="28" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="5"/>
-      <c r="L16" s="64"/>
+      <c r="L16" s="60"/>
     </row>
     <row r="17" spans="1:14" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="27"/>
@@ -5320,16 +5134,16 @@
       <c r="D17" s="45"/>
       <c r="E17" s="8"/>
       <c r="F17" s="27" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G17" s="28" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="5"/>
-      <c r="L17" s="64" t="s">
+      <c r="L17" s="60" t="s">
         <v>85</v>
       </c>
     </row>
@@ -5340,16 +5154,16 @@
       <c r="D18" s="45"/>
       <c r="E18" s="8"/>
       <c r="F18" s="27" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="G18" s="28" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="5"/>
-      <c r="L18" s="64"/>
+      <c r="L18" s="60"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
@@ -5369,7 +5183,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C20" s="31"/>
       <c r="D20" s="31"/>
@@ -5460,18 +5274,18 @@
       </c>
       <c r="J24" s="4"/>
       <c r="K24" s="5"/>
-      <c r="L24" s="49" t="s">
+      <c r="L24" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="M24" s="50"/>
-      <c r="N24" s="51"/>
+      <c r="M24" s="49"/>
+      <c r="N24" s="50"/>
     </row>
     <row r="25" spans="1:14" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="27">
         <v>2</v>
       </c>
       <c r="B25" s="39" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C25" s="40"/>
       <c r="D25" s="39" t="s">
@@ -5488,23 +5302,27 @@
       </c>
       <c r="J25" s="4"/>
       <c r="K25" s="5"/>
-      <c r="L25" s="49" t="s">
+      <c r="L25" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="M25" s="50"/>
-      <c r="N25" s="51"/>
+      <c r="M25" s="49"/>
+      <c r="N25" s="50"/>
     </row>
     <row r="26" spans="1:14" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="27">
         <v>3</v>
       </c>
       <c r="B26" s="39" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C26" s="40"/>
-      <c r="D26" s="39"/>
+      <c r="D26" s="39" t="s">
+        <v>52</v>
+      </c>
       <c r="E26" s="39"/>
-      <c r="F26" s="28"/>
+      <c r="F26" s="28" t="s">
+        <v>52</v>
+      </c>
       <c r="G26" s="4"/>
       <c r="H26" s="5"/>
       <c r="I26" s="42" t="s">
@@ -5512,23 +5330,27 @@
       </c>
       <c r="J26" s="4"/>
       <c r="K26" s="5"/>
-      <c r="L26" s="49" t="s">
+      <c r="L26" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="M26" s="50"/>
-      <c r="N26" s="51"/>
+      <c r="M26" s="49"/>
+      <c r="N26" s="50"/>
     </row>
     <row r="27" spans="1:14" ht="119.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="27">
         <v>4</v>
       </c>
       <c r="B27" s="39" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C27" s="40"/>
-      <c r="D27" s="39"/>
+      <c r="D27" s="39" t="s">
+        <v>54</v>
+      </c>
       <c r="E27" s="39"/>
-      <c r="F27" s="28"/>
+      <c r="F27" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="G27" s="4"/>
       <c r="H27" s="5"/>
       <c r="I27" s="42" t="s">
@@ -5536,26 +5358,26 @@
       </c>
       <c r="J27" s="4"/>
       <c r="K27" s="5"/>
-      <c r="L27" s="49" t="s">
+      <c r="L27" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="M27" s="50"/>
-      <c r="N27" s="51"/>
+      <c r="M27" s="49"/>
+      <c r="N27" s="50"/>
     </row>
     <row r="28" spans="1:14" ht="97.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="27">
         <v>5</v>
       </c>
       <c r="B28" s="39" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C28" s="40"/>
       <c r="D28" s="39" t="s">
-        <v>54</v>
+        <v>192</v>
       </c>
       <c r="E28" s="39"/>
       <c r="F28" s="28" t="s">
-        <v>54</v>
+        <v>192</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="5"/>
@@ -5564,11 +5386,11 @@
       </c>
       <c r="J28" s="4"/>
       <c r="K28" s="5"/>
-      <c r="L28" s="49" t="s">
+      <c r="L28" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="M28" s="50"/>
-      <c r="N28" s="51"/>
+      <c r="M28" s="49"/>
+      <c r="N28" s="50"/>
     </row>
     <row r="29" spans="1:14" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="27">
@@ -5579,11 +5401,11 @@
       </c>
       <c r="C29" s="40"/>
       <c r="D29" s="39" t="s">
-        <v>54</v>
+        <v>193</v>
       </c>
       <c r="E29" s="39"/>
       <c r="F29" s="28" t="s">
-        <v>54</v>
+        <v>193</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="5"/>
@@ -5592,11 +5414,11 @@
       </c>
       <c r="J29" s="4"/>
       <c r="K29" s="5"/>
-      <c r="L29" s="49" t="s">
+      <c r="L29" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="M29" s="50"/>
-      <c r="N29" s="51"/>
+      <c r="M29" s="49"/>
+      <c r="N29" s="50"/>
     </row>
     <row r="30" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="27">
@@ -5607,11 +5429,11 @@
       </c>
       <c r="C30" s="40"/>
       <c r="D30" s="39" t="s">
-        <v>68</v>
+        <v>191</v>
       </c>
       <c r="E30" s="39"/>
       <c r="F30" s="28" t="s">
-        <v>68</v>
+        <v>197</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="5"/>
@@ -5620,11 +5442,11 @@
       </c>
       <c r="J30" s="4"/>
       <c r="K30" s="5"/>
-      <c r="L30" s="49" t="s">
+      <c r="L30" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="M30" s="50"/>
-      <c r="N30" s="51"/>
+      <c r="M30" s="49"/>
+      <c r="N30" s="50"/>
     </row>
     <row r="31" spans="1:14" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="27">
@@ -5635,11 +5457,11 @@
       </c>
       <c r="C31" s="40"/>
       <c r="D31" s="39" t="s">
-        <v>68</v>
+        <v>196</v>
       </c>
       <c r="E31" s="39"/>
       <c r="F31" s="28" t="s">
-        <v>68</v>
+        <v>196</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="5"/>
@@ -5648,240 +5470,80 @@
       </c>
       <c r="J31" s="4"/>
       <c r="K31" s="5"/>
-      <c r="L31" s="49" t="s">
+      <c r="L31" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="M31" s="50"/>
-      <c r="N31" s="51"/>
+      <c r="M31" s="49"/>
+      <c r="N31" s="50"/>
     </row>
     <row r="32" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="27">
         <v>9</v>
       </c>
       <c r="B32" s="39" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C32" s="40"/>
-      <c r="D32" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="E32" s="39"/>
+      <c r="D32" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="E32" s="5"/>
       <c r="F32" s="28" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="5"/>
-      <c r="I32" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="J32" s="4"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="M32" s="50"/>
-      <c r="N32" s="51"/>
+      <c r="I32" s="46" t="s">
+        <v>91</v>
+      </c>
+      <c r="J32" s="57"/>
+      <c r="K32" s="58"/>
+      <c r="L32" s="48" t="s">
+        <v>198</v>
+      </c>
+      <c r="M32" s="49"/>
+      <c r="N32" s="50"/>
     </row>
     <row r="33" spans="1:14" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="27">
         <v>10</v>
       </c>
       <c r="B33" s="39" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C33" s="40"/>
-      <c r="D33" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="E33" s="39"/>
+      <c r="D33" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="E33" s="5"/>
       <c r="F33" s="28" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="5"/>
-      <c r="I33" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="J33" s="4"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="M33" s="50"/>
-      <c r="N33" s="51"/>
-    </row>
-    <row r="34" spans="1:14" ht="67.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="27">
-        <v>11</v>
-      </c>
-      <c r="B34" s="39" t="s">
-        <v>151</v>
-      </c>
-      <c r="C34" s="40"/>
-      <c r="D34" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="E34" s="39"/>
-      <c r="F34" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="G34" s="4"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="J34" s="4"/>
-      <c r="K34" s="5"/>
-      <c r="L34" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="M34" s="50"/>
-      <c r="N34" s="51"/>
-    </row>
-    <row r="35" spans="1:14" ht="69" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="27">
-        <v>12</v>
-      </c>
-      <c r="B35" s="39" t="s">
-        <v>158</v>
-      </c>
-      <c r="C35" s="40"/>
-      <c r="D35" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="E35" s="39"/>
-      <c r="F35" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="G35" s="4"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="J35" s="4"/>
-      <c r="K35" s="5"/>
-      <c r="L35" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="M35" s="50"/>
-      <c r="N35" s="51"/>
-    </row>
-    <row r="36" spans="1:14" ht="70.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="27">
-        <v>13</v>
-      </c>
-      <c r="B36" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="C36" s="40"/>
-      <c r="D36" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="G36" s="4"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="46" t="s">
+      <c r="I33" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="J36" s="4"/>
-      <c r="K36" s="5"/>
-      <c r="L36" s="46" t="s">
-        <v>94</v>
-      </c>
-      <c r="M36" s="4"/>
-      <c r="N36" s="5"/>
-    </row>
-    <row r="37" spans="1:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="27">
-        <v>14</v>
-      </c>
-      <c r="B37" s="39" t="s">
-        <v>156</v>
-      </c>
-      <c r="C37" s="40"/>
-      <c r="D37" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="E37" s="39"/>
-      <c r="F37" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="G37" s="4"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="46" t="s">
-        <v>91</v>
-      </c>
-      <c r="J37" s="4"/>
-      <c r="K37" s="5"/>
-      <c r="L37" s="46" t="s">
-        <v>95</v>
-      </c>
-      <c r="M37" s="4"/>
-      <c r="N37" s="5"/>
-    </row>
-    <row r="38" spans="1:14" ht="76.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="27">
-        <v>15</v>
-      </c>
-      <c r="B38" s="39" t="s">
-        <v>174</v>
-      </c>
-      <c r="C38" s="40"/>
-      <c r="D38" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="E38" s="39"/>
-      <c r="F38" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="G38" s="4"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="46" t="s">
-        <v>91</v>
-      </c>
-      <c r="J38" s="4"/>
-      <c r="K38" s="5"/>
-      <c r="L38" s="46" t="s">
-        <v>96</v>
-      </c>
-      <c r="M38" s="4"/>
-      <c r="N38" s="5"/>
-    </row>
+      <c r="J33" s="57"/>
+      <c r="K33" s="58"/>
+      <c r="L33" s="48" t="s">
+        <v>198</v>
+      </c>
+      <c r="M33" s="49"/>
+      <c r="N33" s="50"/>
+    </row>
+    <row r="34" spans="1:14" ht="67.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="1:14" ht="69" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:14" ht="70.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:14" ht="76.8" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="113">
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="L37:N37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="I38:K38"/>
-    <mergeCell ref="L38:N38"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="L35:N35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="I36:K36"/>
-    <mergeCell ref="L36:N36"/>
+  <mergeCells count="88">
     <mergeCell ref="B33:C33"/>
     <mergeCell ref="D33:E33"/>
     <mergeCell ref="F33:H33"/>
     <mergeCell ref="I33:K33"/>
     <mergeCell ref="L33:N33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="L34:N34"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="F31:H31"/>
@@ -5973,10 +5635,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L20" sqref="L15:L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5986,10 +5648,9 @@
     <col min="5" max="5" width="19.88671875" customWidth="1"/>
     <col min="6" max="6" width="11.109375" customWidth="1"/>
     <col min="8" max="8" width="15.5546875" customWidth="1"/>
-    <col min="12" max="12" width="26.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6008,7 +5669,7 @@
       <c r="J1" s="4"/>
       <c r="K1" s="5"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -6029,7 +5690,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -6042,7 +5703,7 @@
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>7</v>
       </c>
@@ -6057,7 +5718,7 @@
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -6070,7 +5731,7 @@
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>8</v>
       </c>
@@ -6093,7 +5754,7 @@
       <c r="J6" s="19"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="20"/>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
@@ -6106,7 +5767,7 @@
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="21" t="s">
         <v>13</v>
       </c>
@@ -6127,7 +5788,7 @@
       <c r="J8" s="26"/>
       <c r="K8" s="26"/>
     </row>
-    <row r="9" spans="1:12" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="27">
         <v>1</v>
       </c>
@@ -6138,18 +5799,17 @@
       <c r="D9" s="5"/>
       <c r="E9" s="8"/>
       <c r="F9" s="27" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="5"/>
-      <c r="L9" s="48"/>
-    </row>
-    <row r="10" spans="1:12" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:11" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="27">
         <v>2</v>
       </c>
@@ -6163,18 +5823,17 @@
         <v>27</v>
       </c>
       <c r="G10" s="28" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="5"/>
-      <c r="L10" s="48"/>
-    </row>
-    <row r="11" spans="1:12" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:11" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="27"/>
       <c r="B11" s="28" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="5"/>
@@ -6183,15 +5842,14 @@
         <v>28</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="5"/>
-      <c r="L11" s="48"/>
-    </row>
-    <row r="12" spans="1:12" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:11" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -6204,12 +5862,12 @@
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:12" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C13" s="31"/>
       <c r="D13" s="31"/>
@@ -6221,7 +5879,7 @@
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
     </row>
-    <row r="14" spans="1:12" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="32"/>
       <c r="B14" s="32"/>
       <c r="C14" s="32"/>
@@ -6234,7 +5892,7 @@
       <c r="J14" s="32"/>
       <c r="K14" s="32"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="33" t="s">
         <v>17</v>
       </c>
@@ -6256,11 +5914,8 @@
       </c>
       <c r="J15" s="37"/>
       <c r="K15" s="37"/>
-      <c r="L15" s="62" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="34"/>
       <c r="B16" s="38"/>
       <c r="C16" s="38"/>
@@ -6272,9 +5927,8 @@
       <c r="I16" s="37"/>
       <c r="J16" s="37"/>
       <c r="K16" s="37"/>
-      <c r="L16" s="63"/>
-    </row>
-    <row r="17" spans="1:12" ht="87" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:11" ht="87" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="27">
         <v>1</v>
       </c>
@@ -6296,24 +5950,21 @@
       </c>
       <c r="J17" s="4"/>
       <c r="K17" s="5"/>
-      <c r="L17" s="61" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:11" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="27">
         <v>2</v>
       </c>
       <c r="B18" s="39" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C18" s="40"/>
       <c r="D18" s="39" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E18" s="39"/>
       <c r="F18" s="28" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="5"/>
@@ -6322,24 +5973,21 @@
       </c>
       <c r="J18" s="4"/>
       <c r="K18" s="5"/>
-      <c r="L18" s="61" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:11" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="27">
         <v>3</v>
       </c>
       <c r="B19" s="39" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C19" s="40"/>
       <c r="D19" s="39" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E19" s="39"/>
       <c r="F19" s="28" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="5"/>
@@ -6348,24 +5996,21 @@
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="5"/>
-      <c r="L19" s="61" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:11" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="27">
         <v>4</v>
       </c>
       <c r="B20" s="39" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C20" s="40"/>
       <c r="D20" s="39" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E20" s="39"/>
       <c r="F20" s="28" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="5"/>
@@ -6374,26 +6019,23 @@
       </c>
       <c r="J20" s="4"/>
       <c r="K20" s="5"/>
-      <c r="L20" s="61" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="64.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:12" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:12" ht="119.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:12" ht="97.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:12" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:12" ht="75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:12" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:12" ht="75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:12" ht="73.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:12" ht="67.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:12" ht="69" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:12" ht="70.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    </row>
+    <row r="21" spans="1:11" ht="64.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:11" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:11" ht="119.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:11" ht="97.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:11" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:11" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:11" ht="73.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:11" ht="67.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:11" ht="69" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:11" ht="70.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="33" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="34" ht="76.8" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="43">
+  <mergeCells count="42">
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="F20:H20"/>
@@ -6416,7 +6058,6 @@
     <mergeCell ref="D15:E16"/>
     <mergeCell ref="F15:H16"/>
     <mergeCell ref="I15:K16"/>
-    <mergeCell ref="L15:L16"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="G9:K9"/>
     <mergeCell ref="B10:D10"/>
@@ -6447,8 +6088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6611,10 +6252,10 @@
       <c r="D9" s="5"/>
       <c r="E9" s="8"/>
       <c r="F9" s="27" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -6632,10 +6273,10 @@
       <c r="D10" s="5"/>
       <c r="E10" s="8"/>
       <c r="F10" s="27" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G10" s="28" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -6648,11 +6289,11 @@
       <c r="C11" s="4"/>
       <c r="D11" s="5"/>
       <c r="E11" s="8"/>
-      <c r="F11" s="52" t="s">
-        <v>126</v>
+      <c r="F11" s="51" t="s">
+        <v>123</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -6665,11 +6306,11 @@
       <c r="C12" s="44"/>
       <c r="D12" s="45"/>
       <c r="E12" s="8"/>
-      <c r="F12" s="52" t="s">
-        <v>124</v>
+      <c r="F12" s="51" t="s">
+        <v>121</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -6682,11 +6323,11 @@
       <c r="C13" s="44"/>
       <c r="D13" s="45"/>
       <c r="E13" s="8"/>
-      <c r="F13" s="52" t="s">
-        <v>125</v>
+      <c r="F13" s="51" t="s">
+        <v>122</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
@@ -6700,10 +6341,10 @@
       <c r="D14" s="45"/>
       <c r="E14" s="8"/>
       <c r="F14" s="27" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="G14" s="28" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
@@ -6717,10 +6358,10 @@
       <c r="D15" s="45"/>
       <c r="E15" s="8"/>
       <c r="F15" s="27" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G15" s="28" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
@@ -6734,10 +6375,10 @@
       <c r="D16" s="45"/>
       <c r="E16" s="8"/>
       <c r="F16" s="27" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G16" s="28" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -6751,10 +6392,10 @@
       <c r="D17" s="45"/>
       <c r="E17" s="8"/>
       <c r="F17" s="27" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G17" s="28" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
@@ -6768,10 +6409,10 @@
       <c r="D18" s="45"/>
       <c r="E18" s="8"/>
       <c r="F18" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="G18" s="28" t="s">
         <v>135</v>
-      </c>
-      <c r="G18" s="28" t="s">
-        <v>138</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
@@ -6796,7 +6437,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C20" s="31"/>
       <c r="D20" s="31"/>
@@ -6866,111 +6507,111 @@
       </c>
       <c r="C24" s="40"/>
       <c r="D24" s="39" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E24" s="39"/>
       <c r="F24" s="41" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="5"/>
       <c r="I24" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="J24" s="58"/>
-      <c r="K24" s="59"/>
+      <c r="J24" s="57"/>
+      <c r="K24" s="58"/>
     </row>
     <row r="25" spans="1:11" ht="137.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="27">
         <v>2</v>
       </c>
       <c r="B25" s="39" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C25" s="40"/>
       <c r="D25" s="39" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="41" t="s">
-        <v>150</v>
-      </c>
-      <c r="G25" s="54"/>
-      <c r="H25" s="55"/>
+        <v>147</v>
+      </c>
+      <c r="G25" s="53"/>
+      <c r="H25" s="54"/>
       <c r="I25" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="J25" s="58"/>
-      <c r="K25" s="59"/>
+      <c r="J25" s="57"/>
+      <c r="K25" s="58"/>
     </row>
     <row r="26" spans="1:11" ht="140.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="27">
         <v>3</v>
       </c>
       <c r="B26" s="39" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C26" s="40"/>
       <c r="D26" s="28" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="41" t="s">
-        <v>150</v>
-      </c>
-      <c r="G26" s="54"/>
-      <c r="H26" s="55"/>
+        <v>147</v>
+      </c>
+      <c r="G26" s="53"/>
+      <c r="H26" s="54"/>
       <c r="I26" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="J26" s="58"/>
-      <c r="K26" s="59"/>
+      <c r="J26" s="57"/>
+      <c r="K26" s="58"/>
     </row>
     <row r="27" spans="1:11" ht="136.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="27">
         <v>4</v>
       </c>
       <c r="B27" s="39" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C27" s="40"/>
       <c r="D27" s="39" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="41" t="s">
-        <v>150</v>
-      </c>
-      <c r="G27" s="54"/>
-      <c r="H27" s="55"/>
+        <v>147</v>
+      </c>
+      <c r="G27" s="53"/>
+      <c r="H27" s="54"/>
       <c r="I27" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="J27" s="58"/>
-      <c r="K27" s="59"/>
+      <c r="J27" s="57"/>
+      <c r="K27" s="58"/>
     </row>
     <row r="28" spans="1:11" ht="145.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="27">
         <v>5</v>
       </c>
       <c r="B28" s="39" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C28" s="40"/>
       <c r="D28" s="39" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="41" t="s">
-        <v>150</v>
-      </c>
-      <c r="G28" s="54"/>
-      <c r="H28" s="55"/>
+        <v>147</v>
+      </c>
+      <c r="G28" s="53"/>
+      <c r="H28" s="54"/>
       <c r="I28" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="J28" s="58"/>
-      <c r="K28" s="59"/>
+      <c r="J28" s="57"/>
+      <c r="K28" s="58"/>
     </row>
     <row r="29" spans="1:11" ht="136.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="27">
@@ -6981,76 +6622,76 @@
       </c>
       <c r="C29" s="40"/>
       <c r="D29" s="39" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="41" t="s">
-        <v>150</v>
-      </c>
-      <c r="G29" s="54"/>
-      <c r="H29" s="55"/>
+        <v>147</v>
+      </c>
+      <c r="G29" s="53"/>
+      <c r="H29" s="54"/>
       <c r="I29" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="J29" s="58"/>
-      <c r="K29" s="59"/>
+      <c r="J29" s="57"/>
+      <c r="K29" s="58"/>
     </row>
     <row r="30" spans="1:11" ht="79.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="27">
         <v>7</v>
       </c>
       <c r="B30" s="39" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C30" s="40"/>
       <c r="D30" s="28" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="41" t="s">
-        <v>150</v>
-      </c>
-      <c r="G30" s="54"/>
-      <c r="H30" s="55"/>
+        <v>147</v>
+      </c>
+      <c r="G30" s="53"/>
+      <c r="H30" s="54"/>
       <c r="I30" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="J30" s="58"/>
-      <c r="K30" s="59"/>
+      <c r="J30" s="57"/>
+      <c r="K30" s="58"/>
     </row>
     <row r="31" spans="1:11" ht="137.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="27">
         <v>8</v>
       </c>
       <c r="B31" s="39" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C31" s="40"/>
       <c r="D31" s="28" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="41" t="s">
-        <v>150</v>
-      </c>
-      <c r="G31" s="54"/>
-      <c r="H31" s="55"/>
+        <v>147</v>
+      </c>
+      <c r="G31" s="53"/>
+      <c r="H31" s="54"/>
       <c r="I31" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="J31" s="58"/>
-      <c r="K31" s="59"/>
+      <c r="J31" s="57"/>
+      <c r="K31" s="58"/>
     </row>
     <row r="32" spans="1:11" ht="118.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="27">
         <v>9</v>
       </c>
       <c r="B32" s="39" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C32" s="40"/>
       <c r="D32" s="28" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="28" t="s">
@@ -7061,26 +6702,26 @@
       <c r="I32" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="J32" s="58"/>
-      <c r="K32" s="59"/>
+      <c r="J32" s="57"/>
+      <c r="K32" s="58"/>
     </row>
     <row r="33" spans="1:11" ht="135.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="27">
         <v>10</v>
       </c>
       <c r="B33" s="39" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C33" s="40"/>
       <c r="D33" s="39" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="41" t="s">
-        <v>150</v>
-      </c>
-      <c r="G33" s="54"/>
-      <c r="H33" s="55"/>
+        <v>147</v>
+      </c>
+      <c r="G33" s="53"/>
+      <c r="H33" s="54"/>
       <c r="I33" s="46" t="s">
         <v>91</v>
       </c>
@@ -7092,15 +6733,15 @@
         <v>11</v>
       </c>
       <c r="B34" s="39" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C34" s="40"/>
       <c r="D34" s="39" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="28" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="5"/>
@@ -7115,18 +6756,18 @@
         <v>12</v>
       </c>
       <c r="B35" s="39" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C35" s="40"/>
       <c r="D35" s="39" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="41" t="s">
-        <v>150</v>
-      </c>
-      <c r="G35" s="54"/>
-      <c r="H35" s="55"/>
+        <v>147</v>
+      </c>
+      <c r="G35" s="53"/>
+      <c r="H35" s="54"/>
       <c r="I35" s="46" t="s">
         <v>91</v>
       </c>
@@ -7138,19 +6779,19 @@
         <v>13</v>
       </c>
       <c r="B36" s="39" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C36" s="40"/>
       <c r="D36" s="39" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="41" t="s">
-        <v>162</v>
-      </c>
-      <c r="G36" s="54"/>
-      <c r="H36" s="55"/>
-      <c r="I36" s="60" t="s">
+        <v>159</v>
+      </c>
+      <c r="G36" s="53"/>
+      <c r="H36" s="54"/>
+      <c r="I36" s="59" t="s">
         <v>12</v>
       </c>
       <c r="J36" s="4"/>
@@ -7418,13 +7059,13 @@
         <v>1</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="5"/>
-      <c r="O9" s="53"/>
+      <c r="O9" s="52"/>
     </row>
     <row r="10" spans="1:15" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="27"/>
@@ -7436,13 +7077,13 @@
         <v>2</v>
       </c>
       <c r="G10" s="28" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="5"/>
-      <c r="O10" s="53"/>
+      <c r="O10" s="52"/>
     </row>
     <row r="11" spans="1:15" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="27">
@@ -7458,7 +7099,7 @@
         <v>3</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -7475,7 +7116,7 @@
         <v>4</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -7500,7 +7141,7 @@
         <v>16</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C14" s="31"/>
       <c r="D14" s="31"/>
@@ -7570,11 +7211,11 @@
       </c>
       <c r="C18" s="40"/>
       <c r="D18" s="39" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E18" s="39"/>
       <c r="F18" s="41" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="5"/>
@@ -7593,11 +7234,11 @@
       </c>
       <c r="C19" s="40"/>
       <c r="D19" s="28" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="28" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="5"/>
@@ -7616,11 +7257,11 @@
       </c>
       <c r="C20" s="40"/>
       <c r="D20" s="28" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="28" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="5"/>
@@ -7639,34 +7280,34 @@
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="28" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="28" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="5"/>
       <c r="I21" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="J21" s="56"/>
-      <c r="K21" s="57"/>
+      <c r="J21" s="55"/>
+      <c r="K21" s="56"/>
     </row>
     <row r="22" spans="1:11" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="27">
         <v>5</v>
       </c>
       <c r="B22" s="39" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C22" s="40"/>
       <c r="D22" s="39" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E22" s="39"/>
       <c r="F22" s="28" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="5"/>

</xml_diff>